<commit_message>
update information to learn about websocket with esp8266
</commit_message>
<xml_diff>
--- a/PMQLSX/QLSX.xlsx
+++ b/PMQLSX/QLSX.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\A_TDF\Laptrinh\PMQLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Jupiter\PMQLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8749557F-80E0-4908-BD60-4D6263B5030C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="15" windowWidth="20370" windowHeight="10905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="20" windowWidth="20370" windowHeight="10910" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Infos" sheetId="1" r:id="rId1"/>
     <sheet name="MAY" sheetId="2" r:id="rId2"/>
+    <sheet name="ARDUINO" sheetId="3" r:id="rId3"/>
+    <sheet name="ManHinh" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Làm phần mềm quản lý Sản xuất</t>
   </si>
@@ -119,16 +120,138 @@
   </si>
   <si>
     <t>Máy</t>
+  </si>
+  <si>
+    <t>Nhiệm vụ của phần Arduino</t>
+  </si>
+  <si>
+    <t>http://arduino.vn/bai-viet/1496-esp8266-ket-noi-internet-phan-1-cai-dat-esp8266-lam-mot-socket-client-ket-noi-toi</t>
+  </si>
+  <si>
+    <t>ESP8266 kết nối Internet - Phần 1: Cài đặt ESP8266 làm một socket client kết nối tới socket server trong mạng LAN</t>
+  </si>
+  <si>
+    <t>ESP8266 kết nối Internet - Phần 2: Arduino gặp ESP8266, hai đứa nói chuyện bằng JSON</t>
+  </si>
+  <si>
+    <t>http://arduino.vn/bai-viet/1497-esp8266-ket-noi-internet-phan-2-arduino-gap-esp8266-hai-dua-noi-chuyen-bang-json</t>
+  </si>
+  <si>
+    <t>http://arduino.vn/bai-viet/1511-esp8266-ket-noi-internet-phan-3-arduino-gap-smartphone-hai-dua-noi-chuyen-bang-json</t>
+  </si>
+  <si>
+    <t>ESP8266 kết nối Internet - Phần 3: Arduino gặp Smartphone, hai đứa nói chuyện bằng JSON thông qua Socket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kết nối internet </t>
+  </si>
+  <si>
+    <t>http://arduino.vn/bai-viet/1172-lap-trinh-esp8266-bang-arduino-ide</t>
+  </si>
+  <si>
+    <t>Lập trình ESP8266 bằng Arduino IDE</t>
+  </si>
+  <si>
+    <t>http://arduino.vn/bai-viet/1219-tap-lenh-voi-esp8266</t>
+  </si>
+  <si>
+    <t>Tập lệnh AT với ESP8266</t>
+  </si>
+  <si>
+    <t>http://arduino.vn/bai-viet/1171-dieu-khien-thiet-bi-qua-web-sever-voi-esp8266-khong-can-arduino</t>
+  </si>
+  <si>
+    <t>Điều khiển thiết bị qua Web Sever với ESP8266 không cần Arduino</t>
+  </si>
+  <si>
+    <t>2 thông tin cần nhận</t>
+  </si>
+  <si>
+    <t>Công tắc hành trình - để đếm số lần nhấn (có thể sử dụng 2 CTHT để đếm chính xác: 1 cái ở đầu, 1 cái khi kết thúc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mạch tích hợp đầy đủ nguồn </t>
+  </si>
+  <si>
+    <t>Các dây tín hiệu đc nối với domino</t>
+  </si>
+  <si>
+    <t>Chống nhiễu trong mạch, và phần dây tín hiệu nối với CTHT</t>
+  </si>
+  <si>
+    <t>Ghi thông tin vào file .csv - UTF-8</t>
+  </si>
+  <si>
+    <t>Nguồn 24v của đèn báo dừng - khi nào có điện, ko nào tắt điện (có thể test bằng nguồn riêng)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lteGQrY5Yu4</t>
+  </si>
+  <si>
+    <t>ESP8266 IoT Control and Monitor From Anywhere With Arduino and Python | Home Automation</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fREqfdCphRA</t>
+  </si>
+  <si>
+    <t>WebSockets + ESP8266 | a Tutorial for Beginners + Code</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OJIoFtOrXNs&amp;list=PLq1zl76OthiPkemArvlVV2pzp5So0LC_j&amp;index=10</t>
+  </si>
+  <si>
+    <t>TBĐC thông minh: 10. Python và MQTT</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AFz9D9-BQ64</t>
+  </si>
+  <si>
+    <t>[Flutter ESP8266] #1. Gửi và nhận dữ liệu đến ESP8266 (NodeMCU) bằng websocket</t>
+  </si>
+  <si>
+    <t>WebServer trên Esp8266 #1 Dựng Server- Học Cơ Điện Tử</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=R2hqIpvA7zY&amp;list=PL14WBbXTfR-4X5K_JqbLlO3txcmG8pZ4f</t>
+  </si>
+  <si>
+    <t>[tkinter bài 1] Tạo cửa sổ cơ bản - Ngôi Nhà IoT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thông tin có ích cho việc tạo màn hình </t>
+  </si>
+  <si>
+    <t>Thông tin có ích cho việc sử dụng arduino kết nối internet thông qua ESP8266</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Hj_mC6Is2B8&amp;list=PL14WBbXTfR-46Io9ZkdpImV9Ozrct6YPk&amp;index=11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-7-2022 Tìm tài liệu đã tạm ổn - tiến hành làm thôi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">websocket trước </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tạo màn hình </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,13 +274,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -623,106 +749,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>17</v>
       </c>
@@ -733,61 +859,61 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CC328C-DD4E-45A3-B7AB-BFB1D4161F93}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -802,4 +928,201 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G7" r:id="rId5"/>
+    <hyperlink ref="G9" r:id="rId6"/>
+    <hyperlink ref="G11" r:id="rId7"/>
+    <hyperlink ref="G12" r:id="rId8"/>
+    <hyperlink ref="G14" r:id="rId9"/>
+    <hyperlink ref="G16" r:id="rId10"/>
+    <hyperlink ref="G18" r:id="rId11"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
clear files unnecessary - only data store
</commit_message>
<xml_diff>
--- a/PMQLSX/QLSX.xlsx
+++ b/PMQLSX/QLSX.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30" yWindow="20" windowWidth="20370" windowHeight="10910" activeTab="1"/>
+    <workbookView xWindow="30" yWindow="20" windowWidth="20370" windowHeight="10910" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Infos" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Làm phần mềm quản lý Sản xuất</t>
   </si>
@@ -250,6 +250,21 @@
   </si>
   <si>
     <t>Tính năng lịch sử sửa máy: 50k/máy</t>
+  </si>
+  <si>
+    <t>[Unit 9] Socket programming</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-Fs6wAV7tEw</t>
+  </si>
+  <si>
+    <t>Socket</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LWdynDo5jqo</t>
+  </si>
+  <si>
+    <t>[Đồ án mạng máy tính] Share 1: Làm quen với Python socket</t>
   </si>
 </sst>
 </file>
@@ -878,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -948,10 +963,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1086,12 +1101,31 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.35">
       <c r="G18" s="1" t="s">
         <v>65</v>
       </c>
       <c r="H18" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="G21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1107,6 +1141,8 @@
     <hyperlink ref="G14" r:id="rId9"/>
     <hyperlink ref="G16" r:id="rId10"/>
     <hyperlink ref="G18" r:id="rId11"/>
+    <hyperlink ref="G20" r:id="rId12"/>
+    <hyperlink ref="G21" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update infor into excel files
</commit_message>
<xml_diff>
--- a/PMQLSX/QLSX.xlsx
+++ b/PMQLSX/QLSX.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Làm phần mềm quản lý Sản xuất</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>P8 Thêm thư viện arduino cho Wemos D1 để có thể lập trình wemos D1 với Arduino IDE</t>
+  </si>
+  <si>
+    <t>mqtt</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -981,10 +984,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1100,10 +1103,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1168,6 +1174,11 @@
       </c>
       <c r="H25" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data sanluong 13-7-22
</commit_message>
<xml_diff>
--- a/PMQLSX/QLSX.xlsx
+++ b/PMQLSX/QLSX.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
   <si>
     <t>Làm phần mềm quản lý Sản xuất</t>
   </si>
@@ -196,9 +196,6 @@
     <t>https://www.youtube.com/watch?v=fREqfdCphRA</t>
   </si>
   <si>
-    <t>WebSockets + ESP8266 | a Tutorial for Beginners + Code</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=OJIoFtOrXNs&amp;list=PLq1zl76OthiPkemArvlVV2pzp5So0LC_j&amp;index=10</t>
   </si>
   <si>
@@ -295,10 +292,40 @@
     <t>te^34TH24KJd</t>
   </si>
   <si>
-    <t>test_esp</t>
-  </si>
-  <si>
-    <t>ngayhomnay</t>
+    <t>https://console.hivemq.cloud/</t>
+  </si>
+  <si>
+    <t>WebSockets + ESP8266 | Hướng dẫn dành cho người mới bắt đầu + Mã</t>
+  </si>
+  <si>
+    <t>ngoinhaiot.com</t>
+  </si>
+  <si>
+    <t>jhf&amp;623HGb</t>
+  </si>
+  <si>
+    <t>TDSOCK2022</t>
+  </si>
+  <si>
+    <t>http://hivemq.com/demos/websocket-client/</t>
+  </si>
+  <si>
+    <t>Kết nối demo với 1 server khác</t>
+  </si>
+  <si>
+    <t>const char* ssid = "cafe La_Kai";</t>
+  </si>
+  <si>
+    <t>const char* password = "0123456789";</t>
+  </si>
+  <si>
+    <t>const char* mqtt_server = "broker.mqttdashboard.com";</t>
+  </si>
+  <si>
+    <t>Buổi 5/5: ESP32 Client giao thức MQTT, Smart Config</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qxn4haZ6014</t>
   </si>
 </sst>
 </file>
@@ -923,10 +950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,7 +966,7 @@
         <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1020,7 +1047,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>52</v>
@@ -1031,93 +1058,104 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" t="s">
-        <v>55</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" t="s">
         <v>58</v>
       </c>
-      <c r="H16" t="s">
-        <v>59</v>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="G17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.35">
       <c r="G18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.35">
       <c r="F20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.35">
       <c r="G21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" t="s">
         <v>77</v>
-      </c>
-      <c r="H21" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="23" spans="6:8" x14ac:dyDescent="0.35">
       <c r="G23" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="G24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="6:8" x14ac:dyDescent="0.35">
       <c r="G25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" t="s">
         <v>83</v>
-      </c>
-      <c r="H25" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="27" spans="6:8" x14ac:dyDescent="0.35">
       <c r="F27" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="G28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="G30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1129,15 +1167,16 @@
     <hyperlink ref="G7" r:id="rId5"/>
     <hyperlink ref="G9" r:id="rId6"/>
     <hyperlink ref="G11" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="G14" r:id="rId9"/>
-    <hyperlink ref="G16" r:id="rId10"/>
-    <hyperlink ref="G18" r:id="rId11"/>
-    <hyperlink ref="G20" r:id="rId12"/>
-    <hyperlink ref="G21" r:id="rId13"/>
-    <hyperlink ref="G23" r:id="rId14"/>
-    <hyperlink ref="G24" r:id="rId15"/>
-    <hyperlink ref="G25" r:id="rId16"/>
+    <hyperlink ref="G27" r:id="rId8"/>
+    <hyperlink ref="G16" r:id="rId9"/>
+    <hyperlink ref="G18" r:id="rId10"/>
+    <hyperlink ref="G20" r:id="rId11"/>
+    <hyperlink ref="G21" r:id="rId12"/>
+    <hyperlink ref="G23" r:id="rId13"/>
+    <hyperlink ref="G28" r:id="rId14"/>
+    <hyperlink ref="G25" r:id="rId15"/>
+    <hyperlink ref="G17" r:id="rId16"/>
+    <hyperlink ref="G30" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1227,15 +1266,15 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
         <v>61</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1248,33 +1287,71 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C3"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
         <v>86</v>
       </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>89</v>
       </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1290,27 +1367,27 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 30-7-22: giao tiep Serial3 RXD3/TXD3 qua MQTT
</commit_message>
<xml_diff>
--- a/PMQLSX/QLSX.xlsx
+++ b/PMQLSX/QLSX.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30" yWindow="20" windowWidth="20370" windowHeight="10910" activeTab="6"/>
+    <workbookView xWindow="30" yWindow="20" windowWidth="20370" windowHeight="10910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Infos" sheetId="1" r:id="rId1"/>
-    <sheet name="ARDUINO" sheetId="3" r:id="rId2"/>
-    <sheet name="MAY" sheetId="2" r:id="rId3"/>
-    <sheet name="ManHinh" sheetId="4" r:id="rId4"/>
-    <sheet name="MQTT" sheetId="6" r:id="rId5"/>
-    <sheet name="MEGAESP" sheetId="7" r:id="rId6"/>
-    <sheet name="FEE" sheetId="5" r:id="rId7"/>
+    <sheet name="TienDo" sheetId="8" r:id="rId2"/>
+    <sheet name="ARDUINO" sheetId="3" r:id="rId3"/>
+    <sheet name="MAY" sheetId="2" r:id="rId4"/>
+    <sheet name="ManHinh" sheetId="4" r:id="rId5"/>
+    <sheet name="MQTT" sheetId="6" r:id="rId6"/>
+    <sheet name="MEGAESP" sheetId="7" r:id="rId7"/>
+    <sheet name="FEE" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="156">
   <si>
     <t>Làm phần mềm quản lý Sản xuất</t>
   </si>
@@ -480,6 +481,24 @@
   </si>
   <si>
     <t>Còn đoạn đường rất xa mới nghĩ tới vấn đề này đc, cố lên</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qutUNuySdMc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2Hgm8VkpUlw</t>
+  </si>
+  <si>
+    <t>Mega 2560 nhận dữ liệu từ cảm biến độ ẩm truyền qua ESP và sau đó truyền lên Server =&gt; đúng ý mình</t>
+  </si>
+  <si>
+    <t>Nếu mà sử dụng Serial3 thì bật qua RXD3/TXD3 để nạp (nạp chạy được nên chưa thử trường hợp để RXD0/TXD0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đã nạp được code trên MEGA+WiFi R3, truyền nhận dữ liệu các chân qua cổng giao tiếp RXD3/TXD3 và truyền thông qua mạng dùng MQTT, python là nơi xuất ra màn hình </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ra chân và gắn thử vào 10 máy thực tế để kiểm tra số liệu (tình trạng máy -on,off- sau đó sẽ gắn biến đếm SL vào), sau đó sẽ sử dụng JSON để chuẩn hóa dữ liệu </t>
   </si>
 </sst>
 </file>
@@ -524,10 +543,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1105,10 +1125,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>44771</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1394,7 +1452,17 @@
       </c>
     </row>
     <row r="43" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="G43" s="1"/>
+      <c r="G43" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="G44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H44" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1418,12 +1486,13 @@
     <hyperlink ref="G32" r:id="rId18"/>
     <hyperlink ref="G34" r:id="rId19"/>
     <hyperlink ref="G42" r:id="rId20"/>
+    <hyperlink ref="G44" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1495,7 +1564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:E2"/>
   <sheetViews>
@@ -1526,12 +1595,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1622,12 +1691,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1635,37 +1704,37 @@
     <col min="2" max="2" width="58.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>131</v>
       </c>
@@ -1673,7 +1742,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C11">
         <v>1</v>
       </c>
@@ -1696,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>133</v>
       </c>
@@ -1722,7 +1791,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>136</v>
       </c>
@@ -1748,7 +1817,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>137</v>
       </c>
@@ -1773,8 +1842,11 @@
       <c r="I14" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>138</v>
       </c>
@@ -1800,7 +1872,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>139</v>
       </c>
@@ -1920,12 +1992,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
so do mach va ghi chu lai trong file qlsx
</commit_message>
<xml_diff>
--- a/PMQLSX/QLSX.xlsx
+++ b/PMQLSX/QLSX.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30" yWindow="20" windowWidth="20370" windowHeight="10910" activeTab="1"/>
+    <workbookView xWindow="30" yWindow="20" windowWidth="20370" windowHeight="10910" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Infos" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="157">
   <si>
     <t>Làm phần mềm quản lý Sản xuất</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ra chân và gắn thử vào 10 máy thực tế để kiểm tra số liệu (tình trạng máy -on,off- sau đó sẽ gắn biến đếm SL vào), sau đó sẽ sử dụng JSON để chuẩn hóa dữ liệu </t>
+  </si>
+  <si>
+    <t>hàn mạch hơi chuối, nút bấm vào thì thông, bỏ ra thì đứt mạch (đáng lẻ ko cần nút bấm), thêm cái là dây vào không ăn nhập nút bấm và cũng ko ăn nhập luôn pin digital, làm loạn xạ</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1149,9 +1152,17 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
+        <v>44773</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
         <v>44771</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1496,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1568,9 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>